<commit_message>
POL-3113: Trucking issues resolved for v2 (#2507)
* POL-3113: not fast enough

* POL-3113: rewriting coodinate parser

* POL-3113: nearly there

* POL-3113: nearly done

* POL-3113: fixed. needs specs for all three types

* POL-3113: totally working. Need a few more specs

* POL-3113: skip deprecated v2 tests

* POL-3113: fixed and specced

* POL-3113: rubocop and coverage

* POL-3113: last rubocop

* POL-3113: reveted v2 specs chages
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/excel/example_distance_trucking.xlsx
+++ b/spec/fixtures/files/excel/example_distance_trucking.xlsx
@@ -35,7 +35,7 @@
     <t>COUNTRY_CODE</t>
   </si>
   <si>
-    <t>0 - 100</t>
+    <t>0 - 5</t>
   </si>
   <si>
     <t>DE</t>
@@ -5272,14 +5272,30 @@
       <c r="B7" s="19">
         <v>0.0</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="28"/>
+      <c r="C7" s="22">
+        <v>28.392</v>
+      </c>
+      <c r="D7" s="23">
+        <v>35.49</v>
+      </c>
+      <c r="E7" s="24">
+        <v>45.422</v>
+      </c>
+      <c r="F7" s="23">
+        <v>56.069</v>
+      </c>
+      <c r="G7" s="24">
+        <v>71.69500000000001</v>
+      </c>
+      <c r="H7" s="23">
+        <v>79.495</v>
+      </c>
+      <c r="I7" s="25">
+        <v>240.0</v>
+      </c>
+      <c r="J7" s="26">
+        <v>150.0</v>
+      </c>
       <c r="K7" s="29"/>
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>

</xml_diff>